<commit_message>
Further updates on ressurection families. Will now sequence 895 families
</commit_message>
<xml_diff>
--- a/Planning/resurrection_complete.xlsx
+++ b/Planning/resurrection_complete.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Carberry Creek</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Total Refresh</t>
   </si>
   <si>
@@ -273,6 +270,12 @@
   </si>
   <si>
     <t>Just Timeseires</t>
+  </si>
+  <si>
+    <t>All Timeseries</t>
+  </si>
+  <si>
+    <t>Total Sequencing</t>
   </si>
 </sst>
 </file>
@@ -806,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E39256E-CAC5-884D-9652-ED3F0C922410}">
-  <dimension ref="A1:Q72"/>
+  <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="D52" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,7 +848,7 @@
         <v>25</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>24</v>
@@ -978,7 +981,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="15">
         <v>41.296900000000001</v>
@@ -1002,7 +1005,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="15">
         <v>41.228470000000002</v>
@@ -1024,7 +1027,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="15">
         <v>41.250239999999998</v>
@@ -1046,7 +1049,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="15">
         <v>40.43141</v>
@@ -1070,7 +1073,7 @@
         <v>50</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="15">
         <v>39.740009999999998</v>
@@ -1094,7 +1097,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="15">
         <v>40.658270000000002</v>
@@ -1116,7 +1119,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="15">
         <v>40.769959999999998</v>
@@ -1138,7 +1141,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="15">
         <v>40.734311111111097</v>
@@ -1160,7 +1163,7 @@
         <v>53</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="15">
         <v>40.748927777777801</v>
@@ -1182,7 +1185,7 @@
         <v>51</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="15">
         <v>39.99982</v>
@@ -1206,7 +1209,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="15">
         <v>38.928809999999999</v>
@@ -1230,7 +1233,7 @@
         <v>46</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="15">
         <v>39.122050000000002</v>
@@ -1254,7 +1257,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="15">
         <v>38.679879999999997</v>
@@ -1278,7 +1281,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="15">
         <v>38.785400000000003</v>
@@ -1302,7 +1305,7 @@
         <v>69</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="15">
         <v>38.066380000000002</v>
@@ -1324,7 +1327,7 @@
         <v>68</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="15">
         <v>37.89761</v>
@@ -1346,7 +1349,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="15">
         <v>38.069499999999998</v>
@@ -1368,7 +1371,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="15">
         <v>37.743000000000002</v>
@@ -1392,7 +1395,7 @@
         <v>26</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="15">
         <v>37.359200000000001</v>
@@ -1416,7 +1419,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" s="26">
         <v>37.17324</v>
@@ -1438,7 +1441,7 @@
         <v>75</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" s="26">
         <v>35.510809999999999</v>
@@ -1460,7 +1463,7 @@
         <v>66</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="26">
         <v>34.458019999999998</v>
@@ -1475,7 +1478,7 @@
         <v>2</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1484,7 +1487,7 @@
         <v>67</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="26">
         <v>34.490049999999997</v>
@@ -1506,7 +1509,7 @@
         <v>74</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="26">
         <v>34.463590000000003</v>
@@ -1528,7 +1531,7 @@
         <v>83</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="23">
         <f>33+ 40.46/60</f>
@@ -1552,7 +1555,7 @@
         <v>62</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="26">
         <v>33.29533</v>
@@ -1574,7 +1577,7 @@
         <v>79</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="23">
         <f>34 +4.72/60</f>
@@ -1598,7 +1601,7 @@
         <v>80</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="23">
         <f>34 +5.116/60</f>
@@ -1622,7 +1625,7 @@
         <v>77</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="23">
         <f>34 +10.633/60</f>
@@ -1646,7 +1649,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D35" s="23">
         <f>33 +(40.93/60)</f>
@@ -1670,7 +1673,7 @@
         <v>56</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D36" s="15">
         <v>41.87876</v>
@@ -1694,7 +1697,7 @@
         <v>6</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" s="15">
         <v>38.566949999999999</v>
@@ -1762,7 +1765,7 @@
         <v>87</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="15">
         <v>32.801220000000001</v>
@@ -1826,7 +1829,7 @@
         <v>89</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42" s="15">
         <v>33.035960000000003</v>
@@ -1875,7 +1878,7 @@
         <v>91</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D44" s="15">
         <v>34.065109999999997</v>
@@ -1984,7 +1987,7 @@
         <v>94</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D47" s="15">
         <v>34.284970000000001</v>
@@ -2005,7 +2008,7 @@
         <v>95</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D48" s="15">
         <v>34.771709999999999</v>
@@ -2144,7 +2147,7 @@
         <v>99</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D52" s="15">
         <v>37.157609999999998</v>
@@ -2240,7 +2243,7 @@
         <v>102</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" s="15">
         <v>38.3872</v>
@@ -2334,7 +2337,7 @@
         <v>105</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D58" s="15">
         <v>39.553840000000001</v>
@@ -2561,7 +2564,7 @@
         <v>111</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D64" s="15">
         <v>43.413699999999999</v>
@@ -2582,7 +2585,7 @@
         <v>112</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="15">
         <v>43.413699999999999</v>
@@ -2603,7 +2606,7 @@
         <v>113</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D66" s="23">
         <f>33+ 58.961/60</f>
@@ -2628,7 +2631,7 @@
         <v>114</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="15">
         <v>37.776899999999998</v>
@@ -2649,7 +2652,7 @@
         <v>115</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D68" s="15">
         <v>37.818800000000003</v>
@@ -2716,20 +2719,29 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F71" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G71" s="39">
-        <f>SUM(L49:Q49,M51:O51,M53,O53:Q53,N56:Q56,M60:O60,Q60,O61:Q61,M62:Q62,M63,O63:Q63,M69,O69:Q69)</f>
-        <v>230</v>
+        <f>SUM(L41:O41,L45,L46,N45,O46:Q46,P45:Q45,L49:Q49,M51:O51,M53,O53:Q53,N56:Q56,M60:O60,Q60,O61:Q63,M62:N62,M63,M69,O69:Q69)</f>
+        <v>307</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F72" s="38" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="G72" s="39">
+        <f>SUM(K41:O41,K45:L46,N45,O46:Q46,P45:Q45,K49:Q49,L51:O51,K53,M53,O53:R53,K56,N56:Q56,K60,M60:O60,Q60,L61,O61:Q63,K62:K63,M62:N62,M63,K69,M69,O69:Q69)</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F73" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G73" s="39">
         <f>SUM(G70:G71)</f>
-        <v>818</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>